<commit_message>
fixed some warnings and regenerated
</commit_message>
<xml_diff>
--- a/data/cost_delay.xlsx
+++ b/data/cost_delay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oburdash\dev\repos\standard_inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DD202B-0C0D-434E-9E4B-CE16B69CE89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AD75C8-4E57-4E0D-87D2-69429F80571A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tactical" sheetId="1" r:id="rId1"/>
@@ -209,12 +209,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,15 +538,15 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -561,47 +557,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>165.90523690773068</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>45.031421446384037</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>182.49576059850375</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>61.621945137157105</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>212.1216957605985</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>88.877805486284288</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>206.19650872817954</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>84.137655860349128</v>
       </c>
     </row>
@@ -616,15 +612,15 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -632,27 +628,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>17.775561097256858</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>46.690473815461345</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>82.952618453865341</v>
       </c>
     </row>
@@ -666,12 +662,12 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -712,618 +708,618 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>82.952618453865341</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>522.60149625935162</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>1900.8</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>154.05486284289276</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>724.05785536159601</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>2304.8977556109726</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>285.59401496259352</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2">
         <v>1128.1556109725686</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>3111.908229426434</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2">
         <v>261.89326683291773</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2">
         <v>1057.0533665835412</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2">
         <v>2981.5541147132171</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>94.802992518703235</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>593.70374064837904</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>2161.5082294264339</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>177.75561097256858</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>843.74663341645885</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3">
         <v>2672.2593516209477</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>297.44438902743144</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3">
         <v>1199.2578553615961</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3">
         <v>3385.6518703241895</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3">
         <v>297.44438902743144</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3">
         <v>1187.4074812967581</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3">
         <v>3350.1007481296756</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>118.50374064837905</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>688.5067331670823</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>2565.6059850374063</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>201.45635910224439</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>926.69925187032413</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>3040.8059850374066</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <v>356.69625935162094</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>1413.7496259351622</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4">
         <v>4014.9067331670822</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4">
         <v>332.99551122194515</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4">
         <v>1342.6473815461347</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4">
         <v>3872.7022443890273</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>213.30673316708229</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>1175.5571072319201</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>4217.5481296758107</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>404.09775561097257</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>1721.8593516209476</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>5310.1526184538652</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>676.65635910224444</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5">
         <v>2541.9052369077308</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5">
         <v>6960.9097256857858</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5">
         <v>558.15261845386533</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5">
         <v>2185.2089775561099</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5">
         <v>6236.8518703241898</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>35.551122194513717</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>213.30673316708229</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>724.05785536159601</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>71.102244389027433</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>309.29476309226931</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>914.84887780548627</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <v>82.952618453865341</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6">
         <v>344.84588528678302</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6">
         <v>985.95112219451369</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6">
         <v>82.952618453865341</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6">
         <v>344.84588528678302</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6">
         <v>985.95112219451369</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>47.401496259351617</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>285.59401496259352</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>974.10074812967582</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>82.952618453865341</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7">
         <v>392.24738154613465</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <v>1199.2578553615961</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7">
         <v>106.65336658354114</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7">
         <v>463.34962593516207</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7">
         <v>1342.6473815461347</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7">
         <v>106.65336658354114</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7">
         <v>439.64887780548628</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7">
         <v>1295.2458852867831</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>82.952618453865341</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>510.7511221945137</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>1841.5481296758105</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>165.90523690773068</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8">
         <v>748.94364089775559</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>2316.7481296758106</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8">
         <v>297.44438902743144</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8">
         <v>1140.0059850374064</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8">
         <v>3111.908229426434</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8">
         <v>250.04289276807981</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8">
         <v>1009.6518703241895</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8">
         <v>2851.2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>94.802992518703235</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>570.00299251870319</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>2066.7052369077305</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9">
         <v>177.75561097256858</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9">
         <v>820.045885286783</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>2577.4563591022443</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9">
         <v>309.29476309226931</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9">
         <v>1199.2578553615961</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9">
         <v>3326.4</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9">
         <v>297.44438902743144</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9">
         <v>1163.7067331670823</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9">
         <v>3243.4473815461347</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>82.952618453865341</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>463.34962593516207</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>1662.6074812967581</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10">
         <v>165.90523690773068</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10">
         <v>712.20748129675815</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>2149.6578553615959</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10">
         <v>273.7436408977556</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10">
         <v>1045.2029925187032</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10">
         <v>2815.6488778054863</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10">
         <v>213.30673316708229</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10">
         <v>879.29775561097256</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10">
         <v>2482.6533665835414</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>106.65336658354114</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>641.10523690773073</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>2304.8977556109726</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11">
         <v>177.75561097256858</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11">
         <v>855.59700748129671</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11">
         <v>2744.5466334164589</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11">
         <v>321.14513715710723</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11">
         <v>1283.3955112219451</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11">
         <v>3598.9586034912718</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11">
         <v>297.44438902743144</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11">
         <v>1211.1082294264338</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11">
         <v>3456.7541147132169</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>285.59401496259352</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>1627.0563591022444</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <v>5939.4074812967583</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12">
         <v>546.30224438902746</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12">
         <v>2399.700748129676</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12">
         <v>7483.5112219451375</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12">
         <v>1104.4548628428927</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12">
         <v>4086.0089775561096</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12">
         <v>10857.312718204488</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12">
         <v>843.74663341645885</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12">
         <v>3278.9985037406482</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12">
         <v>9242.106733167082</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>118.50374064837905</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>735.90822942643388</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>2719.6608478802991</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13">
         <v>237.0074812967581</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13">
         <v>1092.6044887780549</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13">
         <v>3444.903740648379</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13">
         <v>404.09775561097257</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13">
         <v>1591.5052369077307</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13">
         <v>4430.8548628428925</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13">
         <v>344.84588528678302</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13">
         <v>1401.8992518703242</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13">
         <v>4062.3082294264341</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>201.45635910224439</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>1068.903740648379</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>3801.6</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14">
         <v>344.84588528678302</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14">
         <v>1496.7022443890273</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14">
         <v>4656.0119700748128</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14">
         <v>605.5541147132169</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14">
         <v>2281.1970074812966</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14">
         <v>6225.0014962593514</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14">
         <v>570.00299251870319</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14">
         <v>2173.3586034912719</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14">
         <v>6022.3600997506237</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
         <v>47.401496259351617</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>297.44438902743144</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
         <v>1057.0533665835412</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15">
         <v>82.952618453865341</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15">
         <v>404.09775561097257</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15">
         <v>1271.5451371571073</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15">
         <v>130.35411471321694</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15">
         <v>534.45187032418949</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15">
         <v>1520.4029925187033</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15">
         <v>130.35411471321694</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15">
         <v>534.45187032418949</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15">
         <v>1520.4029925187033</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <v>71.102244389027433</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>380.39700748129678</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
         <v>1366.3481296758105</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16">
         <v>130.35411471321694</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16">
         <v>558.15261845386533</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16">
         <v>1721.8593516209476</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16">
         <v>213.30673316708229</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16">
         <v>831.89625935162098</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16">
         <v>2269.3466334164586</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16">
         <v>213.30673316708229</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16">
         <v>820.045885286783</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16">
         <v>2233.7955112219452</v>
       </c>
     </row>
@@ -1337,16 +1333,16 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1360,213 +1356,213 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>962.25037406483796</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>2281.1970074812966</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>4062.3082294264341</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>1068.903740648379</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>2565.6059850374063</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>4145.2608478802995</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>1247.8443890274314</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>2756.3970074812969</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>4906.0548628428924</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>2043.0044887780548</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>5036.4089775561097</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>8576.115710723192</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>273.7436408977556</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>891.14812967581042</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>1068.903740648379</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>404.09775561097257</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>1163.7067331670823</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>1508.5526184538653</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>641.10523690773073</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>2031.154114713217</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>3801.6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>712.20748129675815</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>2220.7600997506233</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>3908.2533665835413</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>605.5541147132169</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>2031.154114713217</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>3504.1556109725684</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>1199.2578553615961</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>2458.9526184538654</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>4336.0518703241896</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>1782.2962593516208</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>5892.0059850374064</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <v>13006.970573566085</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>855.59700748129671</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>2839.3496259351623</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>5000.8578553615962</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>1555.954114713217</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>4014.9067331670822</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>7400.5586034912722</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
         <v>641.10523690773073</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>1354.4977556109725</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
         <v>1936.3511221945137</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <v>914.84887780548627</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>2043.0044887780548</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
         <v>3267.1481296758107</v>
       </c>
     </row>

</xml_diff>